<commit_message>
Connexion à la BDD
j'ai fais la connexion à la base de données et écris les premières fonctions qui me seront utiles plus tard.
</commit_message>
<xml_diff>
--- a/Documents/Planning/PlaningTpi.xlsx
+++ b/Documents/Planning/PlaningTpi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\TPI_ZaiemElias\Documents\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854A55CC-19E7-40E6-931A-FBE685031592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BBF27C-6259-446F-8E1A-1A5A99F4FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanificationPrévisionnel" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t>Analyse cahier des charges</t>
   </si>
@@ -283,6 +283,18 @@
   </si>
   <si>
     <t>Si l'utilisateur a du mal à utiliser le site, il y à une page d'aide.</t>
+  </si>
+  <si>
+    <t>T2.Connexion à la base de données</t>
+  </si>
+  <si>
+    <t>T3.Inscription/Connexion de l'utilisateur</t>
+  </si>
+  <si>
+    <t>T9.Tri par date/like/catégories des productions</t>
+  </si>
+  <si>
+    <t>T8.Modification des productions</t>
   </si>
 </sst>
 </file>
@@ -819,18 +831,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -869,6 +869,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1166,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C107AC-D199-422A-A85C-C60C00490FB5}">
   <dimension ref="A1:AT34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
@@ -1179,152 +1191,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="78" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78" t="s">
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78" t="s">
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78" t="s">
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78" t="s">
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="78"/>
-      <c r="AG1" s="78"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="78" t="s">
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="78"/>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78" t="s">
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="78" t="s">
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="91"/>
+      <c r="AQ1" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="78"/>
+      <c r="AR1" s="91"/>
+      <c r="AS1" s="91"/>
+      <c r="AT1" s="91"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81">
+      <c r="A2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="94">
         <v>44683</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81">
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94">
         <v>44684</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81">
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94">
         <v>44685</v>
       </c>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81">
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94">
         <v>44686</v>
       </c>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="84">
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="80">
         <v>44690</v>
       </c>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84">
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80">
         <v>44691</v>
       </c>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84">
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+      <c r="AA2" s="80">
         <v>44692</v>
       </c>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84">
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="80"/>
+      <c r="AE2" s="80">
         <v>44693</v>
       </c>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84">
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="80"/>
+      <c r="AH2" s="80"/>
+      <c r="AI2" s="80">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="84">
+      <c r="AJ2" s="80"/>
+      <c r="AK2" s="80"/>
+      <c r="AL2" s="80"/>
+      <c r="AM2" s="80">
         <v>44698</v>
       </c>
-      <c r="AN2" s="84"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="84"/>
-      <c r="AQ2" s="84">
+      <c r="AN2" s="80"/>
+      <c r="AO2" s="80"/>
+      <c r="AP2" s="80"/>
+      <c r="AQ2" s="80">
         <v>44699</v>
       </c>
-      <c r="AR2" s="84"/>
-      <c r="AS2" s="84"/>
-      <c r="AT2" s="84"/>
+      <c r="AR2" s="80"/>
+      <c r="AS2" s="80"/>
+      <c r="AT2" s="80"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
       <c r="E3" s="24"/>
@@ -1471,10 +1483,10 @@
       <c r="AT5" s="7"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="88"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="6"/>
       <c r="D6" s="11"/>
       <c r="E6" s="6"/>
@@ -1671,10 +1683,10 @@
       <c r="AT9" s="7"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="90"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="6"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6"/>
@@ -1871,10 +1883,10 @@
       <c r="AT13" s="7"/>
     </row>
     <row r="14" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="92"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6"/>
@@ -2671,10 +2683,10 @@
       <c r="AT29" s="18"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="94"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="6"/>
       <c r="D30" s="11"/>
       <c r="E30" s="6"/>
@@ -2821,10 +2833,10 @@
       <c r="AT32" s="31"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="83"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="6"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6"/>
@@ -2922,19 +2934,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
@@ -2951,6 +2950,19 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2961,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E298A0-EFFE-4D9D-B5C0-C54E3008405E}">
   <dimension ref="A1:AT34"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2994,152 +3006,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="78" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78" t="s">
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78" t="s">
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78" t="s">
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78" t="s">
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="78"/>
-      <c r="AG1" s="78"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="78" t="s">
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="78"/>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78" t="s">
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="78" t="s">
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="91"/>
+      <c r="AQ1" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="78"/>
+      <c r="AR1" s="91"/>
+      <c r="AS1" s="91"/>
+      <c r="AT1" s="91"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81">
+      <c r="A2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="94">
         <v>44683</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81">
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94">
         <v>44684</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81">
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94">
         <v>44685</v>
       </c>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81">
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94">
         <v>44686</v>
       </c>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="84">
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="80">
         <v>44690</v>
       </c>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84">
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80">
         <v>44691</v>
       </c>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84">
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+      <c r="AA2" s="80">
         <v>44692</v>
       </c>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84">
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="80"/>
+      <c r="AE2" s="80">
         <v>44693</v>
       </c>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84">
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="80"/>
+      <c r="AH2" s="80"/>
+      <c r="AI2" s="80">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="84">
+      <c r="AJ2" s="80"/>
+      <c r="AK2" s="80"/>
+      <c r="AL2" s="80"/>
+      <c r="AM2" s="80">
         <v>44698</v>
       </c>
-      <c r="AN2" s="84"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="84"/>
-      <c r="AQ2" s="84">
+      <c r="AN2" s="80"/>
+      <c r="AO2" s="80"/>
+      <c r="AP2" s="80"/>
+      <c r="AQ2" s="80">
         <v>44699</v>
       </c>
-      <c r="AR2" s="84"/>
-      <c r="AS2" s="84"/>
-      <c r="AT2" s="84"/>
+      <c r="AR2" s="80"/>
+      <c r="AS2" s="80"/>
+      <c r="AT2" s="80"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="57"/>
       <c r="D3" s="58"/>
       <c r="E3" s="57"/>
@@ -3286,10 +3298,10 @@
       <c r="AT5" s="56"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="88"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="54"/>
       <c r="D6" s="55"/>
       <c r="E6" s="54"/>
@@ -3486,10 +3498,10 @@
       <c r="AT9" s="56"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="90"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="54"/>
       <c r="D10" s="55"/>
       <c r="E10" s="54"/>
@@ -3598,8 +3610,8 @@
       <c r="H12" s="34"/>
       <c r="I12" s="72"/>
       <c r="J12" s="55"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="55"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="54"/>
       <c r="N12" s="56"/>
       <c r="O12" s="54"/>
@@ -3649,7 +3661,7 @@
       <c r="I13" s="62"/>
       <c r="J13" s="55"/>
       <c r="K13" s="54"/>
-      <c r="L13" s="55"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="54"/>
       <c r="N13" s="56"/>
       <c r="O13" s="54"/>
@@ -3788,7 +3800,7 @@
     <row r="16" spans="1:46" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="38" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="55"/>
@@ -3798,8 +3810,8 @@
       <c r="H16" s="55"/>
       <c r="I16" s="62"/>
       <c r="J16" s="55"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="55"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="54"/>
       <c r="N16" s="56"/>
       <c r="O16" s="54"/>
@@ -3838,7 +3850,7 @@
     <row r="17" spans="1:46" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="38" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="C17" s="54"/>
       <c r="D17" s="55"/>
@@ -3850,8 +3862,8 @@
       <c r="J17" s="55"/>
       <c r="K17" s="54"/>
       <c r="L17" s="55"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="56"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="18"/>
       <c r="O17" s="54"/>
       <c r="P17" s="56"/>
       <c r="Q17" s="54"/>
@@ -4000,8 +4012,8 @@
       <c r="J20" s="55"/>
       <c r="K20" s="54"/>
       <c r="L20" s="55"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="56"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="77"/>
       <c r="O20" s="54"/>
       <c r="P20" s="56"/>
       <c r="Q20" s="54"/>
@@ -4050,8 +4062,8 @@
       <c r="J21" s="55"/>
       <c r="K21" s="54"/>
       <c r="L21" s="55"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="56"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="77"/>
       <c r="O21" s="54"/>
       <c r="P21" s="56"/>
       <c r="Q21" s="54"/>
@@ -4088,7 +4100,7 @@
     <row r="22" spans="1:46" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="38" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C22" s="54"/>
       <c r="D22" s="55"/>
@@ -4100,8 +4112,8 @@
       <c r="J22" s="55"/>
       <c r="K22" s="54"/>
       <c r="L22" s="55"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="56"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="77"/>
       <c r="O22" s="54"/>
       <c r="P22" s="56"/>
       <c r="Q22" s="54"/>
@@ -4138,7 +4150,7 @@
     <row r="23" spans="1:46" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="38" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="55"/>
@@ -4401,7 +4413,7 @@
       <c r="K28" s="54"/>
       <c r="L28" s="55"/>
       <c r="M28" s="54"/>
-      <c r="N28" s="56"/>
+      <c r="N28" s="18"/>
       <c r="O28" s="65"/>
       <c r="P28" s="66"/>
       <c r="Q28" s="54"/>
@@ -4448,8 +4460,8 @@
       <c r="H29" s="55"/>
       <c r="I29" s="62"/>
       <c r="J29" s="55"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="17"/>
       <c r="M29" s="54"/>
       <c r="N29" s="56"/>
       <c r="O29" s="54"/>
@@ -4486,10 +4498,10 @@
       <c r="AT29" s="56"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="94"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
       <c r="E30" s="54"/>
@@ -4551,7 +4563,7 @@
       <c r="K31" s="54"/>
       <c r="L31" s="55"/>
       <c r="M31" s="54"/>
-      <c r="N31" s="56"/>
+      <c r="N31" s="74"/>
       <c r="O31" s="54"/>
       <c r="P31" s="55"/>
       <c r="Q31" s="54"/>
@@ -4636,10 +4648,10 @@
       <c r="AT32" s="67"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="83"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="54"/>
       <c r="D33" s="55"/>
       <c r="E33" s="54"/>
@@ -4737,13 +4749,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AA2:AD2"/>
@@ -4758,14 +4771,13 @@
     <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="AI2:AL2"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5072,7 +5084,7 @@
       </c>
       <c r="E58" s="50"/>
     </row>
-    <row r="59" spans="2:5" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="B59" s="41" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Documentation et plan de test
J'ai créer un plan de test, je le testerai quand tout fonctionnera.
</commit_message>
<xml_diff>
--- a/Documents/Planning/PlaningTpi.xlsx
+++ b/Documents/Planning/PlaningTpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\TPI_ZaiemElias\Documents\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BBF27C-6259-446F-8E1A-1A5A99F4FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71336CF-13D5-48DD-A3ED-3EB45BDB0FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,6 +831,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -869,18 +881,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1178,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C107AC-D199-422A-A85C-C60C00490FB5}">
   <dimension ref="A1:AT34"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
@@ -1191,152 +1191,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="91" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91" t="s">
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91" t="s">
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91" t="s">
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91" t="s">
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91" t="s">
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91" t="s">
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="91"/>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="91"/>
-      <c r="AI1" s="91" t="s">
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="91"/>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91"/>
-      <c r="AM1" s="91" t="s">
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="91"/>
-      <c r="AO1" s="91"/>
-      <c r="AP1" s="91"/>
-      <c r="AQ1" s="91" t="s">
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="91"/>
-      <c r="AS1" s="91"/>
-      <c r="AT1" s="91"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81">
         <v>44683</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94">
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81">
         <v>44684</v>
       </c>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94">
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81">
         <v>44685</v>
       </c>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94">
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81">
         <v>44686</v>
       </c>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="80">
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="84">
         <v>44690</v>
       </c>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80">
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84">
         <v>44691</v>
       </c>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="80"/>
-      <c r="AA2" s="80">
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84">
         <v>44692</v>
       </c>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="80">
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84">
         <v>44693</v>
       </c>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="80">
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80">
+      <c r="AJ2" s="84"/>
+      <c r="AK2" s="84"/>
+      <c r="AL2" s="84"/>
+      <c r="AM2" s="84">
         <v>44698</v>
       </c>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="80"/>
-      <c r="AP2" s="80"/>
-      <c r="AQ2" s="80">
+      <c r="AN2" s="84"/>
+      <c r="AO2" s="84"/>
+      <c r="AP2" s="84"/>
+      <c r="AQ2" s="84">
         <v>44699</v>
       </c>
-      <c r="AR2" s="80"/>
-      <c r="AS2" s="80"/>
-      <c r="AT2" s="80"/>
+      <c r="AR2" s="84"/>
+      <c r="AS2" s="84"/>
+      <c r="AT2" s="84"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="82"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
       <c r="E3" s="24"/>
@@ -1483,10 +1483,10 @@
       <c r="AT5" s="7"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="6"/>
       <c r="D6" s="11"/>
       <c r="E6" s="6"/>
@@ -1683,10 +1683,10 @@
       <c r="AT9" s="7"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="86"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="6"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6"/>
@@ -1883,10 +1883,10 @@
       <c r="AT13" s="7"/>
     </row>
     <row r="14" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="88"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6"/>
@@ -2683,10 +2683,10 @@
       <c r="AT29" s="18"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="90"/>
+      <c r="B30" s="94"/>
       <c r="C30" s="6"/>
       <c r="D30" s="11"/>
       <c r="E30" s="6"/>
@@ -2833,10 +2833,10 @@
       <c r="AT32" s="31"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="79"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="6"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6"/>
@@ -2934,6 +2934,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
@@ -2950,19 +2963,6 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2974,7 +2974,7 @@
   <dimension ref="A1:AT34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3006,152 +3006,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="91" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91" t="s">
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91" t="s">
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91" t="s">
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91" t="s">
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91" t="s">
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91" t="s">
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="91"/>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="91"/>
-      <c r="AI1" s="91" t="s">
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="91"/>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91"/>
-      <c r="AM1" s="91" t="s">
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="91"/>
-      <c r="AO1" s="91"/>
-      <c r="AP1" s="91"/>
-      <c r="AQ1" s="91" t="s">
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="91"/>
-      <c r="AS1" s="91"/>
-      <c r="AT1" s="91"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81">
         <v>44683</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94">
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81">
         <v>44684</v>
       </c>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94">
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81">
         <v>44685</v>
       </c>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94">
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81">
         <v>44686</v>
       </c>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="80">
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="84">
         <v>44690</v>
       </c>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80">
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84">
         <v>44691</v>
       </c>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="80"/>
-      <c r="AA2" s="80">
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84">
         <v>44692</v>
       </c>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="80">
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84">
         <v>44693</v>
       </c>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="80">
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80">
+      <c r="AJ2" s="84"/>
+      <c r="AK2" s="84"/>
+      <c r="AL2" s="84"/>
+      <c r="AM2" s="84">
         <v>44698</v>
       </c>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="80"/>
-      <c r="AP2" s="80"/>
-      <c r="AQ2" s="80">
+      <c r="AN2" s="84"/>
+      <c r="AO2" s="84"/>
+      <c r="AP2" s="84"/>
+      <c r="AQ2" s="84">
         <v>44699</v>
       </c>
-      <c r="AR2" s="80"/>
-      <c r="AS2" s="80"/>
-      <c r="AT2" s="80"/>
+      <c r="AR2" s="84"/>
+      <c r="AS2" s="84"/>
+      <c r="AT2" s="84"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="82"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="57"/>
       <c r="D3" s="58"/>
       <c r="E3" s="57"/>
@@ -3298,10 +3298,10 @@
       <c r="AT5" s="56"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="54"/>
       <c r="D6" s="55"/>
       <c r="E6" s="54"/>
@@ -3498,10 +3498,10 @@
       <c r="AT9" s="56"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="86"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="54"/>
       <c r="D10" s="55"/>
       <c r="E10" s="54"/>
@@ -4498,10 +4498,10 @@
       <c r="AT29" s="56"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="90"/>
+      <c r="B30" s="94"/>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
       <c r="E30" s="54"/>
@@ -4648,10 +4648,10 @@
       <c r="AT32" s="67"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="79"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="54"/>
       <c r="D33" s="55"/>
       <c r="E33" s="54"/>
@@ -4749,14 +4749,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AA2:AD2"/>
@@ -4771,13 +4770,14 @@
     <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="AI2:AL2"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Planning et journal de bords mis à jour
</commit_message>
<xml_diff>
--- a/Documents/Planning/PlaningTpi.xlsx
+++ b/Documents/Planning/PlaningTpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\TPI_ZaiemElias\Documents\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF32902-8295-4DBE-9F46-5E6EA4C3F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901CC8B-BB77-4214-81C2-0146881A060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,6 +835,18 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -873,18 +885,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1195,152 +1195,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="93" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93" t="s">
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93" t="s">
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93" t="s">
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93" t="s">
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93" t="s">
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93" t="s">
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93" t="s">
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93" t="s">
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="93"/>
-      <c r="AO1" s="93"/>
-      <c r="AP1" s="93"/>
-      <c r="AQ1" s="93" t="s">
+      <c r="AN1" s="80"/>
+      <c r="AO1" s="80"/>
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="80"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83">
         <v>44683</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83">
         <v>44684</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96">
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83">
         <v>44685</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96">
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83">
         <v>44686</v>
       </c>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="82">
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="86">
         <v>44690</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82">
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86">
         <v>44691</v>
       </c>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82">
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86"/>
+      <c r="AA2" s="86">
         <v>44692</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82">
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86">
         <v>44693</v>
       </c>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82">
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="86">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="82"/>
-      <c r="AM2" s="82">
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86">
         <v>44698</v>
       </c>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82">
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+      <c r="AQ2" s="86">
         <v>44699</v>
       </c>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
-      <c r="AT2" s="82"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
       <c r="E3" s="24"/>
@@ -1487,10 +1487,10 @@
       <c r="AT5" s="7"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="6"/>
       <c r="D6" s="11"/>
       <c r="E6" s="6"/>
@@ -1687,10 +1687,10 @@
       <c r="AT9" s="7"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="6"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6"/>
@@ -1887,10 +1887,10 @@
       <c r="AT13" s="7"/>
     </row>
     <row r="14" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="90"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6"/>
@@ -2687,10 +2687,10 @@
       <c r="AT29" s="18"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="92"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="6"/>
       <c r="D30" s="11"/>
       <c r="E30" s="6"/>
@@ -2837,10 +2837,10 @@
       <c r="AT32" s="31"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="81"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="6"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6"/>
@@ -2938,6 +2938,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
@@ -2954,19 +2967,6 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2978,7 +2978,7 @@
   <dimension ref="A1:AT34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="AC18" activeCellId="1" sqref="AD18 AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3010,152 +3010,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="93" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93" t="s">
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93" t="s">
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93" t="s">
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93" t="s">
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93" t="s">
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93" t="s">
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93" t="s">
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93" t="s">
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="93"/>
-      <c r="AO1" s="93"/>
-      <c r="AP1" s="93"/>
-      <c r="AQ1" s="93" t="s">
+      <c r="AN1" s="80"/>
+      <c r="AO1" s="80"/>
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="80"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83">
         <v>44683</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83">
         <v>44684</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96">
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83">
         <v>44685</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96">
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83">
         <v>44686</v>
       </c>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="82">
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="86">
         <v>44690</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82">
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86">
         <v>44691</v>
       </c>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82">
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86"/>
+      <c r="AA2" s="86">
         <v>44692</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82">
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86">
         <v>44693</v>
       </c>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82">
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="86">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="82"/>
-      <c r="AM2" s="82">
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86">
         <v>44698</v>
       </c>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82">
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+      <c r="AQ2" s="86">
         <v>44699</v>
       </c>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
-      <c r="AT2" s="82"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="57"/>
       <c r="D3" s="58"/>
       <c r="E3" s="57"/>
@@ -3302,10 +3302,10 @@
       <c r="AT5" s="56"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="54"/>
       <c r="D6" s="55"/>
       <c r="E6" s="54"/>
@@ -3502,10 +3502,10 @@
       <c r="AT9" s="56"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="54"/>
       <c r="D10" s="55"/>
       <c r="E10" s="54"/>
@@ -3930,14 +3930,14 @@
       <c r="X18" s="56"/>
       <c r="Y18" s="54"/>
       <c r="Z18" s="56"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="54"/>
-      <c r="AD18" s="56"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="56"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="18"/>
       <c r="AE18" s="54"/>
       <c r="AF18" s="55"/>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="56"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="18"/>
       <c r="AI18" s="54"/>
       <c r="AJ18" s="55"/>
       <c r="AK18" s="54"/>
@@ -3981,11 +3981,11 @@
       <c r="Y19" s="54"/>
       <c r="Z19" s="56"/>
       <c r="AA19" s="54"/>
-      <c r="AB19" s="18"/>
+      <c r="AB19" s="56"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="18"/>
-      <c r="AE19" s="54"/>
-      <c r="AF19" s="55"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="17"/>
       <c r="AG19" s="54"/>
       <c r="AH19" s="56"/>
       <c r="AI19" s="54"/>
@@ -4234,8 +4234,8 @@
       <c r="AB24" s="56"/>
       <c r="AC24" s="54"/>
       <c r="AD24" s="56"/>
-      <c r="AE24" s="54"/>
-      <c r="AF24" s="55"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="17"/>
       <c r="AG24" s="54"/>
       <c r="AH24" s="56"/>
       <c r="AI24" s="54"/>
@@ -4437,7 +4437,7 @@
       <c r="AE28" s="54"/>
       <c r="AF28" s="55"/>
       <c r="AG28" s="54"/>
-      <c r="AH28" s="56"/>
+      <c r="AH28" s="18"/>
       <c r="AI28" s="54"/>
       <c r="AJ28" s="55"/>
       <c r="AK28" s="54"/>
@@ -4480,8 +4480,8 @@
       <c r="X29" s="55"/>
       <c r="Y29" s="54"/>
       <c r="Z29" s="18"/>
-      <c r="AA29" s="54"/>
-      <c r="AB29" s="55"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="17"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="18"/>
       <c r="AE29" s="54"/>
@@ -4502,10 +4502,10 @@
       <c r="AT29" s="56"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="92"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
       <c r="E30" s="54"/>
@@ -4652,10 +4652,10 @@
       <c r="AT32" s="67"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="81"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="54"/>
       <c r="D33" s="55"/>
       <c r="E33" s="54"/>
@@ -4753,14 +4753,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AA2:AD2"/>
@@ -4775,13 +4774,14 @@
     <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="AI2:AL2"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Push du 16.05.2022 Après-midi
</commit_message>
<xml_diff>
--- a/Documents/Planning/PlaningTpi.xlsx
+++ b/Documents/Planning/PlaningTpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\TPI_ZaiemElias\Documents\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E006EBEB-23A6-4489-963F-EBA40D1F9873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5138FC-2ED2-4375-915D-8760B3DD6CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,6 +835,21 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -874,26 +889,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1198,152 +1198,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="93" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93" t="s">
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93" t="s">
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93" t="s">
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93" t="s">
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93" t="s">
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93" t="s">
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93" t="s">
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93" t="s">
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
+      <c r="AL1" s="81"/>
+      <c r="AM1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="93"/>
-      <c r="AO1" s="93"/>
-      <c r="AP1" s="93"/>
-      <c r="AQ1" s="93" t="s">
+      <c r="AN1" s="81"/>
+      <c r="AO1" s="81"/>
+      <c r="AP1" s="81"/>
+      <c r="AQ1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
+      <c r="AR1" s="81"/>
+      <c r="AS1" s="81"/>
+      <c r="AT1" s="81"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96">
+      <c r="A2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84">
         <v>44683</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96">
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84">
         <v>44684</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96">
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84">
         <v>44685</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96">
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84">
         <v>44686</v>
       </c>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="82">
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="87">
         <v>44690</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82">
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87">
         <v>44691</v>
       </c>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82">
+      <c r="X2" s="87"/>
+      <c r="Y2" s="87"/>
+      <c r="Z2" s="87"/>
+      <c r="AA2" s="87">
         <v>44692</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82">
+      <c r="AB2" s="87"/>
+      <c r="AC2" s="87"/>
+      <c r="AD2" s="87"/>
+      <c r="AE2" s="87">
         <v>44693</v>
       </c>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82">
+      <c r="AF2" s="87"/>
+      <c r="AG2" s="87"/>
+      <c r="AH2" s="87"/>
+      <c r="AI2" s="87">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="82"/>
-      <c r="AM2" s="82">
+      <c r="AJ2" s="87"/>
+      <c r="AK2" s="87"/>
+      <c r="AL2" s="87"/>
+      <c r="AM2" s="87">
         <v>44698</v>
       </c>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82">
+      <c r="AN2" s="87"/>
+      <c r="AO2" s="87"/>
+      <c r="AP2" s="87"/>
+      <c r="AQ2" s="87">
         <v>44699</v>
       </c>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
-      <c r="AT2" s="82"/>
+      <c r="AR2" s="87"/>
+      <c r="AS2" s="87"/>
+      <c r="AT2" s="87"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
       <c r="E3" s="24"/>
@@ -1490,10 +1490,10 @@
       <c r="AT5" s="7"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="91"/>
       <c r="C6" s="6"/>
       <c r="D6" s="11"/>
       <c r="E6" s="6"/>
@@ -1690,10 +1690,10 @@
       <c r="AT9" s="7"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="6"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6"/>
@@ -1890,10 +1890,10 @@
       <c r="AT13" s="7"/>
     </row>
     <row r="14" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="90"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6"/>
@@ -2690,10 +2690,10 @@
       <c r="AT29" s="18"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="92"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="6"/>
       <c r="D30" s="11"/>
       <c r="E30" s="6"/>
@@ -2840,10 +2840,10 @@
       <c r="AT32" s="31"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="81"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="6"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6"/>
@@ -2941,6 +2941,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
@@ -2957,19 +2970,6 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2980,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E298A0-EFFE-4D9D-B5C0-C54E3008405E}">
   <dimension ref="A1:AT34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM14" sqref="AM14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3013,152 +3013,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="93" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93" t="s">
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93" t="s">
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93" t="s">
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93" t="s">
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93" t="s">
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93" t="s">
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93" t="s">
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="93"/>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93" t="s">
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
+      <c r="AL1" s="81"/>
+      <c r="AM1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="93"/>
-      <c r="AO1" s="93"/>
-      <c r="AP1" s="93"/>
-      <c r="AQ1" s="93" t="s">
+      <c r="AN1" s="81"/>
+      <c r="AO1" s="81"/>
+      <c r="AP1" s="81"/>
+      <c r="AQ1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
+      <c r="AR1" s="81"/>
+      <c r="AS1" s="81"/>
+      <c r="AT1" s="81"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96">
+      <c r="A2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84">
         <v>44683</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96">
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84">
         <v>44684</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96">
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84">
         <v>44685</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96">
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84">
         <v>44686</v>
       </c>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="82">
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="87">
         <v>44690</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82">
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87">
         <v>44691</v>
       </c>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82">
+      <c r="X2" s="87"/>
+      <c r="Y2" s="87"/>
+      <c r="Z2" s="87"/>
+      <c r="AA2" s="87">
         <v>44692</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82">
+      <c r="AB2" s="87"/>
+      <c r="AC2" s="87"/>
+      <c r="AD2" s="87"/>
+      <c r="AE2" s="87">
         <v>44693</v>
       </c>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82">
+      <c r="AF2" s="87"/>
+      <c r="AG2" s="87"/>
+      <c r="AH2" s="87"/>
+      <c r="AI2" s="87">
         <v>44697</v>
       </c>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="82"/>
-      <c r="AM2" s="82">
+      <c r="AJ2" s="87"/>
+      <c r="AK2" s="87"/>
+      <c r="AL2" s="87"/>
+      <c r="AM2" s="87">
         <v>44698</v>
       </c>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="82"/>
-      <c r="AP2" s="82"/>
-      <c r="AQ2" s="82">
+      <c r="AN2" s="87"/>
+      <c r="AO2" s="87"/>
+      <c r="AP2" s="87"/>
+      <c r="AQ2" s="87">
         <v>44699</v>
       </c>
-      <c r="AR2" s="82"/>
-      <c r="AS2" s="82"/>
-      <c r="AT2" s="82"/>
+      <c r="AR2" s="87"/>
+      <c r="AS2" s="87"/>
+      <c r="AT2" s="87"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="57"/>
       <c r="D3" s="58"/>
       <c r="E3" s="57"/>
@@ -3305,10 +3305,10 @@
       <c r="AT5" s="56"/>
     </row>
     <row r="6" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="91"/>
       <c r="C6" s="54"/>
       <c r="D6" s="55"/>
       <c r="E6" s="54"/>
@@ -3505,10 +3505,10 @@
       <c r="AT9" s="56"/>
     </row>
     <row r="10" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="54"/>
       <c r="D10" s="55"/>
       <c r="E10" s="54"/>
@@ -3705,10 +3705,10 @@
       <c r="AT13" s="56"/>
     </row>
     <row r="14" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="98"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="54"/>
       <c r="D14" s="55"/>
       <c r="E14" s="54"/>
@@ -4141,10 +4141,10 @@
       <c r="AF22" s="55"/>
       <c r="AG22" s="54"/>
       <c r="AH22" s="56"/>
-      <c r="AI22" s="54"/>
-      <c r="AJ22" s="55"/>
-      <c r="AK22" s="54"/>
-      <c r="AL22" s="56"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="17"/>
+      <c r="AK22" s="19"/>
+      <c r="AL22" s="18"/>
       <c r="AM22" s="54"/>
       <c r="AN22" s="55"/>
       <c r="AO22" s="54"/>
@@ -4394,7 +4394,7 @@
       <c r="AI27" s="54"/>
       <c r="AJ27" s="55"/>
       <c r="AK27" s="54"/>
-      <c r="AL27" s="56"/>
+      <c r="AL27" s="18"/>
       <c r="AM27" s="54"/>
       <c r="AN27" s="55"/>
       <c r="AO27" s="54"/>
@@ -4444,7 +4444,7 @@
       <c r="AI28" s="54"/>
       <c r="AJ28" s="55"/>
       <c r="AK28" s="54"/>
-      <c r="AL28" s="56"/>
+      <c r="AL28" s="18"/>
       <c r="AM28" s="54"/>
       <c r="AN28" s="55"/>
       <c r="AO28" s="54"/>
@@ -4494,7 +4494,7 @@
       <c r="AI29" s="54"/>
       <c r="AJ29" s="55"/>
       <c r="AK29" s="54"/>
-      <c r="AL29" s="56"/>
+      <c r="AL29" s="18"/>
       <c r="AM29" s="54"/>
       <c r="AN29" s="55"/>
       <c r="AO29" s="54"/>
@@ -4505,10 +4505,10 @@
       <c r="AT29" s="56"/>
     </row>
     <row r="30" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="92"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
       <c r="E30" s="54"/>
@@ -4590,7 +4590,7 @@
       <c r="AE31" s="67"/>
       <c r="AF31" s="68"/>
       <c r="AG31" s="67"/>
-      <c r="AH31" s="99"/>
+      <c r="AH31" s="80"/>
       <c r="AI31" s="67"/>
       <c r="AJ31" s="68"/>
       <c r="AK31" s="70"/>
@@ -4643,8 +4643,8 @@
       <c r="AH32" s="69"/>
       <c r="AI32" s="67"/>
       <c r="AJ32" s="67"/>
-      <c r="AK32" s="67"/>
-      <c r="AL32" s="67"/>
+      <c r="AK32" s="79"/>
+      <c r="AL32" s="79"/>
       <c r="AM32" s="67"/>
       <c r="AN32" s="67"/>
       <c r="AO32" s="54"/>
@@ -4655,10 +4655,10 @@
       <c r="AT32" s="67"/>
     </row>
     <row r="33" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="81"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="54"/>
       <c r="D33" s="55"/>
       <c r="E33" s="54"/>
@@ -4756,14 +4756,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AA2:AD2"/>
@@ -4778,13 +4777,14 @@
     <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="AI2:AL2"/>
     <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>